<commit_message>
page clear 시 dialog 추가 및 max width, 텍스트 줄넘김, 마진 설정
</commit_message>
<xml_diff>
--- a/src/GridaBoard/language/textData.xlsx
+++ b/src/GridaBoard/language/textData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loite\Documents\GridaBoard2\src\GridaBoard\language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388EBFBF-D906-47FD-A906-55D12C78B0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F382AFD-9280-46B4-AFB4-0640CA10F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22740" yWindow="4620" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="string" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="705">
   <si>
     <t>Gridaboard 2.0 string</t>
   </si>
@@ -2153,6 +2153,19 @@
   </si>
   <si>
     <t>Do you want to remove the page?</t>
+    <phoneticPr fontId="40" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리다보드 &gt; 왼쪽 사이드 버튼</t>
+  </si>
+  <si>
+    <t>현재 페이지의 필기를 모두 삭제하시겠습니까?</t>
+  </si>
+  <si>
+    <t>Are you sure you want to delete all of the notes on the current page?</t>
+  </si>
+  <si>
+    <t>clearPage_title</t>
     <phoneticPr fontId="40" type="noConversion"/>
   </si>
 </sst>
@@ -2160,7 +2173,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="43">
+  <fonts count="44">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2399,6 +2412,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Noto Sans KR"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
       <name val="Noto Sans KR"/>
       <family val="2"/>
     </font>
@@ -2763,7 +2782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3151,6 +3170,9 @@
     <xf numFmtId="0" fontId="13" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -3372,10 +3394,10 @@
   <dimension ref="A1:Z1058"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G155" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G146" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G168" sqref="G168"/>
+      <selection pane="bottomRight" activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -9980,14 +10002,24 @@
       <c r="Y168" s="51"/>
       <c r="Z168" s="51"/>
     </row>
-    <row r="169" spans="1:26" ht="14.25">
+    <row r="169" spans="1:26" ht="15" thickBot="1">
       <c r="A169" s="41"/>
       <c r="B169" s="112"/>
-      <c r="C169" s="111"/>
-      <c r="D169" s="110"/>
-      <c r="E169" s="111"/>
-      <c r="F169" s="142"/>
-      <c r="G169" s="126"/>
+      <c r="C169" s="161" t="s">
+        <v>704</v>
+      </c>
+      <c r="D169" s="162" t="s">
+        <v>701</v>
+      </c>
+      <c r="E169" s="161" t="s">
+        <v>683</v>
+      </c>
+      <c r="F169" s="167" t="s">
+        <v>702</v>
+      </c>
+      <c r="G169" s="164" t="s">
+        <v>703</v>
+      </c>
       <c r="H169" s="126"/>
       <c r="I169" s="126"/>
       <c r="J169" s="51"/>

</xml_diff>